<commit_message>
meike added stuff, updating files
</commit_message>
<xml_diff>
--- a/01-getting-started/data/yrbss20.xlsx
+++ b/01-getting-started/data/yrbss20.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t xml:space="preserve">bmi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight</t>
   </si>
   <si>
     <t xml:space="preserve">text_while_driving_30d</t>
@@ -464,77 +467,89 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>335340</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>27.5671</v>
       </c>
-      <c r="G2"/>
+      <c r="G2" t="n">
+        <v>3.1945</v>
+      </c>
       <c r="H2"/>
       <c r="I2"/>
+      <c r="J2"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>638618</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3"/>
       <c r="F3" t="n">
         <v>29.3495</v>
       </c>
-      <c r="G3"/>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3"/>
+      <c r="G3" t="n">
+        <v>1.0206</v>
+      </c>
+      <c r="H3"/>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>922382</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>18.1827</v>
       </c>
-      <c r="G4"/>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="b">
+      <c r="G4" t="n">
+        <v>2.0312</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -543,25 +558,28 @@
         <v>923122</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" t="n">
         <v>21.3754</v>
       </c>
-      <c r="G5"/>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="b">
+      <c r="G5" t="n">
+        <v>0.5954</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -570,25 +588,28 @@
         <v>923963</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F6" t="n">
         <v>19.5988</v>
       </c>
-      <c r="G6"/>
-      <c r="H6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" t="b">
+      <c r="G6" t="n">
+        <v>0.6833</v>
+      </c>
+      <c r="H6"/>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -597,25 +618,28 @@
         <v>925603</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7" t="n">
         <v>22.191</v>
       </c>
-      <c r="G7"/>
-      <c r="H7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" t="b">
+      <c r="G7" t="n">
+        <v>0.8456</v>
+      </c>
+      <c r="H7"/>
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" t="b">
         <v>1</v>
       </c>
     </row>
@@ -624,25 +648,28 @@
         <v>933724</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F8" t="n">
         <v>20.9913</v>
       </c>
-      <c r="G8"/>
-      <c r="H8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" t="b">
+      <c r="G8" t="n">
+        <v>0.4695</v>
+      </c>
+      <c r="H8"/>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -651,25 +678,28 @@
         <v>935435</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
         <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
       </c>
       <c r="F9" t="n">
         <v>17.4814</v>
       </c>
-      <c r="G9"/>
-      <c r="H9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" t="b">
+      <c r="G9" t="n">
+        <v>0.8511</v>
+      </c>
+      <c r="H9"/>
+      <c r="I9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" t="b">
         <v>0</v>
       </c>
     </row>
@@ -678,23 +708,26 @@
         <v>1096564</v>
       </c>
       <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F10" t="n">
         <v>22.4593</v>
       </c>
-      <c r="G10"/>
+      <c r="G10" t="n">
+        <v>1.2463</v>
+      </c>
       <c r="H10"/>
-      <c r="I10" t="b">
+      <c r="I10"/>
+      <c r="J10" t="b">
         <v>1</v>
       </c>
     </row>
@@ -703,25 +736,28 @@
         <v>1108114</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F11" t="n">
         <v>26.5781</v>
       </c>
-      <c r="G11"/>
-      <c r="H11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" t="b">
+      <c r="G11" t="n">
+        <v>0.8134</v>
+      </c>
+      <c r="H11"/>
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" t="b">
         <v>0</v>
       </c>
     </row>
@@ -730,25 +766,28 @@
         <v>1306150</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F12" t="n">
         <v>21.1874</v>
       </c>
-      <c r="G12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12"/>
-      <c r="I12" t="b">
+      <c r="G12" t="n">
+        <v>2.322</v>
+      </c>
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12"/>
+      <c r="J12" t="b">
         <v>0</v>
       </c>
     </row>
@@ -757,27 +796,30 @@
         <v>1307481</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F13" t="n">
         <v>19.4637</v>
       </c>
-      <c r="G13" t="s">
-        <v>25</v>
+      <c r="G13" t="n">
+        <v>0.2678</v>
       </c>
       <c r="H13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" t="b">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -786,27 +828,30 @@
         <v>1307872</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F14" t="n">
         <v>20.6121</v>
       </c>
-      <c r="G14" t="s">
-        <v>25</v>
+      <c r="G14" t="n">
+        <v>0.8173</v>
       </c>
       <c r="H14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" t="b">
+        <v>26</v>
+      </c>
+      <c r="I14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" t="b">
         <v>0</v>
       </c>
     </row>
@@ -815,27 +860,30 @@
         <v>1311617</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F15" t="n">
         <v>27.4648</v>
       </c>
-      <c r="G15" t="s">
-        <v>24</v>
+      <c r="G15" t="n">
+        <v>0.4251</v>
       </c>
       <c r="H15" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" t="b">
+        <v>25</v>
+      </c>
+      <c r="I15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" t="b">
         <v>1</v>
       </c>
     </row>
@@ -844,27 +892,30 @@
         <v>1313153</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F16" t="n">
         <v>26.5781</v>
       </c>
-      <c r="G16" t="s">
-        <v>24</v>
+      <c r="G16" t="n">
+        <v>0.5173</v>
       </c>
       <c r="H16" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" t="b">
+        <v>25</v>
+      </c>
+      <c r="I16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" t="b">
         <v>1</v>
       </c>
     </row>
@@ -873,27 +924,30 @@
         <v>1313291</v>
       </c>
       <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" t="s">
         <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" t="s">
-        <v>12</v>
       </c>
       <c r="F17" t="n">
         <v>24.8047</v>
       </c>
-      <c r="G17" t="s">
-        <v>27</v>
+      <c r="G17" t="n">
+        <v>1.1997</v>
       </c>
       <c r="H17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" t="b">
+        <v>28</v>
+      </c>
+      <c r="I17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" t="b">
         <v>0</v>
       </c>
     </row>
@@ -902,27 +956,30 @@
         <v>1313477</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F18" t="n">
         <v>25.0318</v>
       </c>
-      <c r="G18" t="s">
-        <v>24</v>
+      <c r="G18" t="n">
+        <v>0.9901</v>
       </c>
       <c r="H18" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" t="b">
+        <v>25</v>
+      </c>
+      <c r="I18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" t="b">
         <v>1</v>
       </c>
     </row>
@@ -931,25 +988,28 @@
         <v>1315121</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E19"/>
       <c r="F19" t="n">
         <v>22.2687</v>
       </c>
-      <c r="G19" t="s">
-        <v>28</v>
+      <c r="G19" t="n">
+        <v>4.4926</v>
       </c>
       <c r="H19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" t="b">
+        <v>29</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" t="b">
         <v>0</v>
       </c>
     </row>
@@ -958,25 +1018,28 @@
         <v>1315850</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F20" t="n">
         <v>19.4922</v>
       </c>
-      <c r="G20" t="s">
-        <v>24</v>
-      </c>
-      <c r="H20"/>
-      <c r="I20" t="b">
+      <c r="G20" t="n">
+        <v>0.8376</v>
+      </c>
+      <c r="H20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20"/>
+      <c r="J20" t="b">
         <v>0</v>
       </c>
     </row>
@@ -985,27 +1048,30 @@
         <v>1316123</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F21" t="n">
         <v>27.4894</v>
       </c>
-      <c r="G21" t="s">
-        <v>30</v>
+      <c r="G21" t="n">
+        <v>0.2913</v>
       </c>
       <c r="H21" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" t="b">
+        <v>31</v>
+      </c>
+      <c r="I21" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>